<commit_message>
extend tests as described in RT #79016
</commit_message>
<xml_diff>
--- a/t/3_____invalid_formular.xlsx
+++ b/t/3_____invalid_formular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\root\Documents\GitHub\Spreadsheet-XLSX\t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E22DEE-FAFF-487C-8654-8A1661BF937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E5FBF9-9621-4C3B-B1F0-A64F112C0338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17490" yWindow="270" windowWidth="27840" windowHeight="21495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23565" yWindow="960" windowWidth="27840" windowHeight="21495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,18 +368,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
-        <f>1/0</f>
+        <f>0/0</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="e" cm="1">
+        <f t="array" aca="1" ref="A2" ca="1">_xludf.NA()</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="e">
+        <f>"a"+0</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>